<commit_message>
ejercicio 2 de la leccion 9 listo
</commit_message>
<xml_diff>
--- a/UiPathAcademy/leccion 9/practica1/Sums.xlsx
+++ b/UiPathAcademy/leccion 9/practica1/Sums.xlsx
@@ -331,99 +331,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C9" sqref="C1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>159</v>
+        <v>623</v>
       </c>
       <c r="B1">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3359</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9072</v>
+        <v>6643</v>
       </c>
       <c r="B3">
-        <v>8996</v>
+        <v>88942</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>623</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11</v>
+        <v>3213</v>
       </c>
       <c r="B5">
-        <v>324</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6643</v>
+        <v>7732</v>
       </c>
       <c r="B6">
-        <v>88942</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>952</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3213</v>
+        <v>3577</v>
       </c>
       <c r="B8">
-        <v>4324</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7732</v>
+        <v>3577</v>
       </c>
       <c r="B9">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>952</v>
-      </c>
-      <c r="B10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3577</v>
-      </c>
-      <c r="B11">
         <v>91</v>
       </c>
     </row>

</xml_diff>